<commit_message>
failed test re-tested after fix
</commit_message>
<xml_diff>
--- a/manual-test/Manual-Test.xlsx
+++ b/manual-test/Manual-Test.xlsx
@@ -8,13 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Tanulas\6felev\IET\iet-hf-2024-rovarirtok\manual-test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0CC40A41-7115-44B7-8E4F-B821A967A33A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{060CE46E-46EC-49D9-BB7F-8DB627DDB7FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19090" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="19090" yWindow="-110" windowWidth="19420" windowHeight="11020" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="initial-tests" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
+    <sheet name="failure re-testing" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="119">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="248" uniqueCount="122">
   <si>
     <t>Test #</t>
   </si>
@@ -450,6 +450,15 @@
   </si>
   <si>
     <t>A cső megfelelő vége le lesz csatolva</t>
+  </si>
+  <si>
+    <t>2024.05.13</t>
+  </si>
+  <si>
+    <t>Fixed, bin könyvtárhoz hozzáadva a az assests könyvtár az erőforrásokkal</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fixed </t>
   </si>
 </sst>
 </file>
@@ -550,12 +559,6 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -571,12 +574,32 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Style 1" xfId="1" xr:uid="{168E0B8F-68E8-4629-BFBD-6FBF1FBA428C}"/>
   </cellStyles>
-  <dxfs count="2">
+  <dxfs count="4">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -869,7 +892,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L20"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+    <sheetView topLeftCell="A10" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
       <selection activeCell="A13" sqref="A13:XFD13"/>
     </sheetView>
   </sheetViews>
@@ -918,390 +941,390 @@
       </c>
     </row>
     <row r="2" spans="1:12" ht="123.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="E2" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="F2" s="4" t="s">
+      <c r="F2" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="G2" s="4" t="s">
+      <c r="G2" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="H2" s="4" t="s">
+      <c r="H2" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="I2" s="4" t="s">
+      <c r="I2" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="J2" s="2" t="s">
+      <c r="J2" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="K2" s="5"/>
-      <c r="L2" s="6" t="s">
+      <c r="K2" s="3"/>
+      <c r="L2" s="4" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="3" spans="1:12" ht="123.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="7"/>
-      <c r="B3" s="7"/>
-      <c r="C3" s="7"/>
-      <c r="D3" s="8"/>
-      <c r="E3" s="8"/>
-      <c r="F3" s="5" t="s">
+      <c r="A3" s="5"/>
+      <c r="B3" s="5"/>
+      <c r="C3" s="5"/>
+      <c r="D3" s="6"/>
+      <c r="E3" s="6"/>
+      <c r="F3" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="G3" s="4" t="s">
+      <c r="G3" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="H3" s="4" t="s">
+      <c r="H3" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="I3" s="4" t="s">
+      <c r="I3" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="J3" s="7"/>
-      <c r="K3" s="4" t="s">
+      <c r="J3" s="5"/>
+      <c r="K3" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="L3" s="6" t="s">
+      <c r="L3" s="4" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="4" spans="1:12" ht="123.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="5" t="s">
+      <c r="A4" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="B4" s="5" t="s">
+      <c r="B4" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="C4" s="5" t="s">
+      <c r="C4" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="D4" s="4" t="s">
+      <c r="D4" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="E4" s="4" t="s">
+      <c r="E4" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="F4" s="4" t="s">
+      <c r="F4" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="G4" s="4" t="s">
+      <c r="G4" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="H4" s="4" t="s">
+      <c r="H4" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="I4" s="4" t="s">
+      <c r="I4" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="J4" s="5" t="s">
+      <c r="J4" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="K4" s="4" t="s">
+      <c r="K4" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="L4" s="4" t="s">
+      <c r="L4" s="2" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="5" spans="1:12" ht="123.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="5" t="s">
+      <c r="A5" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="B5" s="5" t="s">
+      <c r="B5" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="C5" s="5" t="s">
+      <c r="C5" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="D5" s="4" t="s">
+      <c r="D5" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="E5" s="4" t="s">
+      <c r="E5" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="F5" s="5" t="s">
+      <c r="F5" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="G5" s="4" t="s">
+      <c r="G5" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="H5" s="4" t="s">
+      <c r="H5" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="I5" s="4" t="s">
+      <c r="I5" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="J5" s="5" t="s">
+      <c r="J5" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="K5" s="5"/>
-      <c r="L5" s="5" t="s">
+      <c r="K5" s="3"/>
+      <c r="L5" s="3" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="6" spans="1:12" ht="123.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="5" t="s">
+      <c r="A6" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="B6" s="4" t="s">
+      <c r="B6" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="C6" s="5" t="s">
+      <c r="C6" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="D6" s="4" t="s">
+      <c r="D6" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="E6" s="4" t="s">
+      <c r="E6" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="F6" s="5" t="s">
+      <c r="F6" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="G6" s="4" t="s">
+      <c r="G6" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="H6" s="4" t="s">
+      <c r="H6" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="I6" s="4" t="s">
+      <c r="I6" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="J6" s="5" t="s">
+      <c r="J6" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="K6" s="5"/>
-      <c r="L6" s="5" t="s">
+      <c r="K6" s="3"/>
+      <c r="L6" s="3" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="7" spans="1:12" ht="123.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="5" t="s">
+      <c r="A7" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="B7" s="4" t="s">
+      <c r="B7" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="C7" s="5" t="s">
+      <c r="C7" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="D7" s="4" t="s">
+      <c r="D7" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="E7" s="4" t="s">
+      <c r="E7" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="F7" s="5" t="s">
+      <c r="F7" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="G7" s="4" t="s">
+      <c r="G7" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="H7" s="4" t="s">
+      <c r="H7" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="I7" s="4" t="s">
+      <c r="I7" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="J7" s="5" t="s">
+      <c r="J7" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="K7" s="5"/>
-      <c r="L7" s="5" t="s">
+      <c r="K7" s="3"/>
+      <c r="L7" s="3" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="8" spans="1:12" ht="123.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="5" t="s">
+      <c r="A8" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="B8" s="4" t="s">
+      <c r="B8" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="C8" s="5" t="s">
+      <c r="C8" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="D8" s="4" t="s">
+      <c r="D8" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="E8" s="4" t="s">
+      <c r="E8" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="F8" s="5" t="s">
+      <c r="F8" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="G8" s="4" t="s">
+      <c r="G8" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="H8" s="4" t="s">
+      <c r="H8" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="I8" s="4" t="s">
+      <c r="I8" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="J8" s="5" t="s">
+      <c r="J8" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="K8" s="5"/>
-      <c r="L8" s="5" t="s">
+      <c r="K8" s="3"/>
+      <c r="L8" s="3" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="9" spans="1:12" ht="123.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="5" t="s">
+      <c r="A9" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="B9" s="4" t="s">
+      <c r="B9" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="C9" s="5" t="s">
+      <c r="C9" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="D9" s="4" t="s">
+      <c r="D9" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="E9" s="4" t="s">
+      <c r="E9" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="F9" s="5" t="s">
+      <c r="F9" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="G9" s="4" t="s">
+      <c r="G9" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="H9" s="4" t="s">
+      <c r="H9" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="I9" s="4" t="s">
+      <c r="I9" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="J9" s="5" t="s">
+      <c r="J9" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="K9" s="5"/>
-      <c r="L9" s="5" t="s">
+      <c r="K9" s="3"/>
+      <c r="L9" s="3" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="10" spans="1:12" ht="123.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="5" t="s">
+      <c r="A10" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="B10" s="5" t="s">
+      <c r="B10" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="C10" s="5" t="s">
+      <c r="C10" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="D10" s="4" t="s">
+      <c r="D10" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="E10" s="4" t="s">
+      <c r="E10" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="F10" s="5" t="s">
+      <c r="F10" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="G10" s="4" t="s">
+      <c r="G10" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="H10" s="4" t="s">
+      <c r="H10" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="I10" s="4" t="s">
+      <c r="I10" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="J10" s="5" t="s">
+      <c r="J10" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="K10" s="5"/>
-      <c r="L10" s="5" t="s">
+      <c r="K10" s="3"/>
+      <c r="L10" s="3" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="11" spans="1:12" ht="123.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="5" t="s">
+      <c r="A11" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="B11" s="5" t="s">
+      <c r="B11" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="C11" s="5" t="s">
+      <c r="C11" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="D11" s="4" t="s">
+      <c r="D11" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="E11" s="4" t="s">
+      <c r="E11" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="F11" s="5" t="s">
+      <c r="F11" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="G11" s="4" t="s">
+      <c r="G11" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="H11" s="4" t="s">
+      <c r="H11" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="I11" s="4" t="s">
+      <c r="I11" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="J11" s="5" t="s">
+      <c r="J11" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="K11" s="5"/>
-      <c r="L11" s="5" t="s">
+      <c r="K11" s="3"/>
+      <c r="L11" s="3" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="12" spans="1:12" ht="123.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="5" t="s">
+      <c r="A12" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="B12" s="5" t="s">
+      <c r="B12" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="C12" s="5" t="s">
+      <c r="C12" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="D12" s="4" t="s">
+      <c r="D12" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="E12" s="4" t="s">
+      <c r="E12" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="F12" s="5" t="s">
+      <c r="F12" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="G12" s="4" t="s">
+      <c r="G12" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="H12" s="4" t="s">
+      <c r="H12" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="I12" s="4" t="s">
+      <c r="I12" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="J12" s="5" t="s">
+      <c r="J12" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="K12" s="5"/>
-      <c r="L12" s="5" t="s">
+      <c r="K12" s="3"/>
+      <c r="L12" s="3" t="s">
         <v>22</v>
       </c>
     </row>
@@ -1344,242 +1367,243 @@
       </c>
     </row>
     <row r="14" spans="1:12" ht="123.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="2" t="s">
+      <c r="A14" s="7" t="s">
         <v>84</v>
       </c>
-      <c r="B14" s="2" t="s">
+      <c r="B14" s="7" t="s">
         <v>85</v>
       </c>
-      <c r="C14" s="2" t="s">
+      <c r="C14" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="D14" s="3" t="s">
+      <c r="D14" s="8" t="s">
         <v>86</v>
       </c>
-      <c r="E14" s="3" t="s">
+      <c r="E14" s="8" t="s">
         <v>87</v>
       </c>
-      <c r="F14" s="5" t="s">
+      <c r="F14" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="G14" s="4" t="s">
+      <c r="G14" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="H14" s="4" t="s">
+      <c r="H14" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="I14" s="4" t="s">
+      <c r="I14" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="J14" s="2" t="s">
+      <c r="J14" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="K14" s="5"/>
-      <c r="L14" s="5" t="s">
+      <c r="K14" s="3"/>
+      <c r="L14" s="3" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="15" spans="1:12" ht="123.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="7"/>
-      <c r="B15" s="7"/>
-      <c r="C15" s="7"/>
-      <c r="D15" s="8"/>
-      <c r="E15" s="8"/>
-      <c r="F15" s="5" t="s">
+      <c r="A15" s="5"/>
+      <c r="B15" s="5"/>
+      <c r="C15" s="5"/>
+      <c r="D15" s="6"/>
+      <c r="E15" s="6"/>
+      <c r="F15" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="G15" s="5" t="s">
+      <c r="G15" s="3" t="s">
         <v>90</v>
       </c>
-      <c r="H15" s="4" t="s">
+      <c r="H15" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="I15" s="4" t="s">
+      <c r="I15" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="J15" s="7"/>
-      <c r="K15" s="5"/>
-      <c r="L15" s="5" t="s">
+      <c r="J15" s="5"/>
+      <c r="K15" s="3"/>
+      <c r="L15" s="3" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="16" spans="1:12" ht="123.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="7" t="s">
+      <c r="A16" s="5" t="s">
         <v>92</v>
       </c>
-      <c r="B16" s="7" t="s">
+      <c r="B16" s="5" t="s">
         <v>93</v>
       </c>
-      <c r="C16" s="7" t="s">
+      <c r="C16" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="D16" s="8" t="s">
+      <c r="D16" s="6" t="s">
         <v>94</v>
       </c>
-      <c r="E16" s="8" t="s">
+      <c r="E16" s="6" t="s">
         <v>95</v>
       </c>
-      <c r="F16" s="5" t="s">
+      <c r="F16" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="G16" s="5" t="s">
+      <c r="G16" s="3" t="s">
         <v>96</v>
       </c>
-      <c r="H16" s="4" t="s">
+      <c r="H16" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="I16" s="4" t="s">
+      <c r="I16" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="J16" s="7" t="s">
+      <c r="J16" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="K16" s="5"/>
-      <c r="L16" s="5" t="s">
+      <c r="K16" s="3"/>
+      <c r="L16" s="3" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="17" spans="1:12" ht="123.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="7"/>
-      <c r="B17" s="7"/>
-      <c r="C17" s="7"/>
-      <c r="D17" s="8"/>
-      <c r="E17" s="8"/>
-      <c r="F17" s="5" t="s">
+      <c r="A17" s="5"/>
+      <c r="B17" s="5"/>
+      <c r="C17" s="5"/>
+      <c r="D17" s="6"/>
+      <c r="E17" s="6"/>
+      <c r="F17" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="G17" s="4" t="s">
+      <c r="G17" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="H17" s="4" t="s">
+      <c r="H17" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="I17" s="4" t="s">
+      <c r="I17" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="J17" s="7"/>
-      <c r="K17" s="4" t="s">
+      <c r="J17" s="5"/>
+      <c r="K17" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="L17" s="5" t="s">
+      <c r="L17" s="3" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="18" spans="1:12" ht="123.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="5" t="s">
+      <c r="A18" s="3" t="s">
         <v>101</v>
       </c>
-      <c r="B18" s="5" t="s">
+      <c r="B18" s="3" t="s">
         <v>102</v>
       </c>
-      <c r="C18" s="5" t="s">
+      <c r="C18" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="D18" s="4" t="s">
+      <c r="D18" s="2" t="s">
         <v>103</v>
       </c>
-      <c r="E18" s="4" t="s">
+      <c r="E18" s="2" t="s">
         <v>104</v>
       </c>
-      <c r="F18" s="5" t="s">
+      <c r="F18" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="G18" s="4" t="s">
+      <c r="G18" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="H18" s="4" t="s">
+      <c r="H18" s="2" t="s">
         <v>106</v>
       </c>
-      <c r="I18" s="4" t="s">
+      <c r="I18" s="2" t="s">
         <v>106</v>
       </c>
-      <c r="J18" s="5" t="s">
+      <c r="J18" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="K18" s="5"/>
-      <c r="L18" s="5" t="s">
+      <c r="K18" s="3"/>
+      <c r="L18" s="3" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="19" spans="1:12" ht="123.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="5" t="s">
+      <c r="A19" s="3" t="s">
         <v>107</v>
       </c>
-      <c r="B19" s="5" t="s">
+      <c r="B19" s="3" t="s">
         <v>108</v>
       </c>
-      <c r="C19" s="5" t="s">
+      <c r="C19" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="D19" s="4" t="s">
+      <c r="D19" s="2" t="s">
         <v>109</v>
       </c>
-      <c r="E19" s="4" t="s">
+      <c r="E19" s="2" t="s">
         <v>110</v>
       </c>
-      <c r="F19" s="5" t="s">
+      <c r="F19" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="G19" s="4" t="s">
+      <c r="G19" s="2" t="s">
         <v>111</v>
       </c>
-      <c r="H19" s="4" t="s">
+      <c r="H19" s="2" t="s">
         <v>112</v>
       </c>
-      <c r="I19" s="4" t="s">
+      <c r="I19" s="2" t="s">
         <v>112</v>
       </c>
-      <c r="J19" s="5" t="s">
+      <c r="J19" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="K19" s="5"/>
-      <c r="L19" s="5" t="s">
+      <c r="K19" s="3"/>
+      <c r="L19" s="3" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="20" spans="1:12" ht="123.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="5" t="s">
+      <c r="A20" s="3" t="s">
         <v>113</v>
       </c>
-      <c r="B20" s="5" t="s">
+      <c r="B20" s="3" t="s">
         <v>114</v>
       </c>
-      <c r="C20" s="5" t="s">
+      <c r="C20" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="D20" s="4" t="s">
+      <c r="D20" s="2" t="s">
         <v>115</v>
       </c>
-      <c r="E20" s="4" t="s">
+      <c r="E20" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="F20" s="5" t="s">
+      <c r="F20" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="G20" s="4" t="s">
+      <c r="G20" s="2" t="s">
         <v>117</v>
       </c>
-      <c r="H20" s="4" t="s">
+      <c r="H20" s="2" t="s">
         <v>118</v>
       </c>
-      <c r="I20" s="4" t="s">
+      <c r="I20" s="2" t="s">
         <v>118</v>
       </c>
-      <c r="J20" s="5" t="s">
+      <c r="J20" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="K20" s="5"/>
-      <c r="L20" s="5" t="s">
+      <c r="K20" s="3"/>
+      <c r="L20" s="3" t="s">
         <v>22</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="18">
-    <mergeCell ref="A16:A17"/>
-    <mergeCell ref="B16:B17"/>
-    <mergeCell ref="C16:C17"/>
-    <mergeCell ref="D16:D17"/>
-    <mergeCell ref="E16:E17"/>
+    <mergeCell ref="J2:J3"/>
+    <mergeCell ref="A2:A3"/>
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="C2:C3"/>
+    <mergeCell ref="D2:D3"/>
+    <mergeCell ref="E2:E3"/>
     <mergeCell ref="J16:J17"/>
     <mergeCell ref="A14:A15"/>
     <mergeCell ref="B14:B15"/>
@@ -1587,6 +1611,174 @@
     <mergeCell ref="D14:D15"/>
     <mergeCell ref="E14:E15"/>
     <mergeCell ref="J14:J15"/>
+    <mergeCell ref="A16:A17"/>
+    <mergeCell ref="B16:B17"/>
+    <mergeCell ref="C16:C17"/>
+    <mergeCell ref="D16:D17"/>
+    <mergeCell ref="E16:E17"/>
+  </mergeCells>
+  <conditionalFormatting sqref="L1:L15 K16:L16 L17:L20">
+    <cfRule type="cellIs" dxfId="3" priority="1" operator="equal">
+      <formula>"FAIL"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="2" priority="2" operator="equal">
+      <formula>"PASS"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8675BD1A-449F-44DD-B8A0-5D27B89A5837}">
+  <dimension ref="A1:L4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="N3" sqref="N3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="17" defaultRowHeight="153" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:12" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" ht="153" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>119</v>
+      </c>
+      <c r="D2" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="E2" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="J2" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="K2" s="3"/>
+      <c r="L2" s="4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" ht="153" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="5"/>
+      <c r="B3" s="6"/>
+      <c r="C3" s="5"/>
+      <c r="D3" s="6"/>
+      <c r="E3" s="6"/>
+      <c r="F3" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="I3" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="J3" s="5"/>
+      <c r="K3" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="L3" s="4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" ht="153" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="I4" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="J4" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="K4" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="L4" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="6">
     <mergeCell ref="A2:A3"/>
     <mergeCell ref="B2:B3"/>
     <mergeCell ref="C2:C3"/>
@@ -1594,7 +1786,7 @@
     <mergeCell ref="E2:E3"/>
     <mergeCell ref="J2:J3"/>
   </mergeCells>
-  <conditionalFormatting sqref="L1:L15 K16:L16 L17:L20">
+  <conditionalFormatting sqref="L1:L4">
     <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
       <formula>"FAIL"</formula>
     </cfRule>
@@ -1604,16 +1796,4 @@
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8675BD1A-449F-44DD-B8A0-5D27B89A5837}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>